<commit_message>
Update Lineux One vzbot330 bom
Update Lineux One vzbot330 bom to include stainless steel solder flux
</commit_message>
<xml_diff>
--- a/BOM/Lineux One Vzbot Bom.xlsx
+++ b/BOM/Lineux One Vzbot Bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
   <si>
     <t>Vzbot Carriage</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>spring OD6 ID5 10mm</t>
+  </si>
+  <si>
+    <t>stainless steel solder flux</t>
+  </si>
+  <si>
+    <t>You will need to sodler wires to the spring which will require this flux</t>
   </si>
   <si>
     <t>Lineux One Toolhead (Bom is for 1 toolhead)</t>
@@ -296,7 +302,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -308,6 +314,11 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -393,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -449,6 +460,9 @@
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
@@ -692,7 +706,7 @@
     <col customWidth="1" min="4" max="4" width="2.38"/>
     <col customWidth="1" min="5" max="5" width="23.5"/>
     <col customWidth="1" min="6" max="6" width="7.25"/>
-    <col customWidth="1" min="7" max="7" width="48.75"/>
+    <col customWidth="1" min="7" max="7" width="50.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -987,603 +1001,599 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="11">
         <v>2.0</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="24">
-      <c r="A24" s="20" t="s">
+    <row r="23">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="C23" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="20" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="7" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="11">
-        <v>4.0</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G27" s="5" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="C28" s="11">
         <v>4.0</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C29" s="11">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F29" s="11">
         <v>1.0</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="G29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C30" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="s">
-        <v>37</v>
+      <c r="A31" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="10" t="s">
         <v>48</v>
       </c>
       <c r="F31" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>49</v>
+        <v>1.0</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="13" t="s">
+      <c r="F32" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F32" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="13" t="s">
-        <v>37</v>
+      <c r="A34" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C34" s="11">
         <v>2.0</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="22"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>24</v>
+      <c r="A35" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="C35" s="11">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="10"/>
-      <c r="F35" s="22"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C36" s="11">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="10"/>
-      <c r="F36" s="22"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37" s="11">
         <v>3.0</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="22"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" s="11">
         <v>3.0</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="10"/>
-      <c r="F38" s="21"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" s="11">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="10"/>
-      <c r="F39" s="21"/>
+      <c r="F39" s="22"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C40" s="11">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="21"/>
+      <c r="F40" s="22"/>
       <c r="G40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41" s="11">
         <v>3.0</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="10"/>
-      <c r="F41" s="21"/>
+      <c r="F41" s="22"/>
       <c r="G41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="11">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="21"/>
+      <c r="F42" s="22"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C43" s="11">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="10"/>
-      <c r="F43" s="21"/>
+      <c r="F43" s="22"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C44" s="11">
         <v>1.0</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="21"/>
+      <c r="F44" s="22"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C45" s="11">
         <v>1.0</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="10"/>
-      <c r="F45" s="21"/>
+      <c r="F45" s="22"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C46" s="11">
         <v>1.0</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="10"/>
-      <c r="F46" s="21"/>
+      <c r="F46" s="22"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="10"/>
-      <c r="F47" s="21"/>
+      <c r="F47" s="22"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="10" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="10" t="s">
-        <v>66</v>
-      </c>
+      <c r="E48" s="10"/>
       <c r="F48" s="22"/>
-      <c r="G48" s="5" t="s">
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>6</v>
+      <c r="B49" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C49" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F49" s="22"/>
+        <v>68</v>
+      </c>
+      <c r="F49" s="23"/>
       <c r="G49" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>71</v>
+      <c r="A50" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="C50" s="11">
         <v>2.0</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" s="23"/>
+      <c r="G50" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="F50" s="22"/>
-      <c r="G50" s="12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C51" s="11">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="5"/>
+      <c r="E51" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="23"/>
+      <c r="G51" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C52" s="11">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="10"/>
-      <c r="F52" s="21"/>
+      <c r="F52" s="22"/>
       <c r="G52" s="5"/>
     </row>
     <row r="53">
-      <c r="A53" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="19">
+      <c r="A53" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="11">
         <v>3.0</v>
       </c>
       <c r="D53" s="5"/>
-      <c r="E53" s="17" t="s">
+      <c r="E53" s="10"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F53" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="G53" s="5"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="B54" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="19">
+        <v>3.0</v>
+      </c>
       <c r="D54" s="5"/>
-      <c r="F54" s="23"/>
+      <c r="E54" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="19">
+        <v>1.0</v>
+      </c>
       <c r="G54" s="5"/>
     </row>
     <row r="55">
-      <c r="A55" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="F55" s="24"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="6" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="7" t="s">
+      <c r="F57" s="4"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B58" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C58" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="7" t="s">
+      <c r="D58" s="5"/>
+      <c r="E58" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F58" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="10"/>
-      <c r="B58" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G58" s="5"/>
+      <c r="G58" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="10"/>
-      <c r="B59" s="12" t="s">
-        <v>8</v>
+      <c r="B59" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C59" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F59" s="11">
         <v>1.0</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="G59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="10"/>
       <c r="B60" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C60" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="10" t="s">
@@ -1592,44 +1602,50 @@
       <c r="F60" s="11">
         <v>1.0</v>
       </c>
-      <c r="G60" s="5"/>
+      <c r="G60" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="10"/>
-      <c r="B61" s="5" t="s">
-        <v>82</v>
+      <c r="B61" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C61" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D61" s="5"/>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F61" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>73</v>
-      </c>
+      <c r="F61" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="G61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="10"/>
       <c r="B62" s="5" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="C62" s="11">
         <v>1.0</v>
       </c>
       <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="5"/>
+      <c r="E62" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F62" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="10"/>
       <c r="B63" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C63" s="11">
         <v>1.0</v>
@@ -1642,62 +1658,62 @@
     <row r="64">
       <c r="A64" s="10"/>
       <c r="B64" s="5" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="C64" s="11">
         <v>1.0</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="F64" s="25"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="10"/>
-      <c r="B65" s="12" t="s">
-        <v>85</v>
+      <c r="B65" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C65" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-      <c r="F65" s="23"/>
+      <c r="F65" s="5"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="10"/>
-      <c r="B66" s="5" t="s">
-        <v>86</v>
+      <c r="B66" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="C66" s="11">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
-      <c r="F66" s="23"/>
+      <c r="F66" s="24"/>
       <c r="G66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="10"/>
       <c r="B67" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C67" s="11">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="F67" s="24"/>
       <c r="G67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="10"/>
       <c r="B68" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C68" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -1707,7 +1723,7 @@
     <row r="69">
       <c r="A69" s="10"/>
       <c r="B69" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C69" s="11">
         <v>2.0</v>
@@ -1720,10 +1736,10 @@
     <row r="70">
       <c r="A70" s="10"/>
       <c r="B70" s="5" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C70" s="11">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -1733,10 +1749,10 @@
     <row r="71">
       <c r="A71" s="10"/>
       <c r="B71" s="5" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C71" s="11">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -1746,7 +1762,7 @@
     <row r="72">
       <c r="A72" s="10"/>
       <c r="B72" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C72" s="11">
         <v>1.0</v>
@@ -1757,11 +1773,11 @@
       <c r="G72" s="5"/>
     </row>
     <row r="73">
-      <c r="A73" s="17"/>
-      <c r="B73" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C73" s="26">
+      <c r="A73" s="10"/>
+      <c r="B73" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" s="11">
         <v>1.0</v>
       </c>
       <c r="D73" s="5"/>
@@ -1769,17 +1785,30 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
     </row>
+    <row r="74">
+      <c r="A74" s="17"/>
+      <c r="B74" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C74" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A56:F56"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Lineux One Bom and CAD
Fix m3 dowel support length
Improved dock rigidity
Updated BOM
</commit_message>
<xml_diff>
--- a/BOM/Lineux One Vzbot Bom.xlsx
+++ b/BOM/Lineux One Vzbot Bom.xlsx
@@ -100,7 +100,7 @@
     <t>m3 x 35mm dowel pin</t>
   </si>
   <si>
-    <t>m3 x 54mm dowel pin</t>
+    <t>m3 x 45mm dowel pin</t>
   </si>
   <si>
     <t>m5 hex nut</t>
@@ -277,7 +277,7 @@
     <t>m3 t nut</t>
   </si>
   <si>
-    <t>m5 x 8mm bhcs</t>
+    <t>m5 x 12mm bhcs</t>
   </si>
   <si>
     <t>m4 x 15mm threaded dowel pin ID m3</t>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="67">
       <c r="A67" s="10"/>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="12" t="s">
         <v>88</v>
       </c>
       <c r="C67" s="11">

</xml_diff>